<commit_message>
Added ROC curves and overview of best hyperparameters
</commit_message>
<xml_diff>
--- a/results/12hr_ensembled.xlsx
+++ b/results/12hr_ensembled.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="183">
   <si>
     <t xml:space="preserve">estimator</t>
   </si>
@@ -1289,6 +1289,237 @@
    micro avg       0.85      0.85      0.85       240
    macro avg       0.86      0.86      0.85       240
 weighted avg       0.86      0.85      0.85       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only the best features:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.83      0.80      0.81       123
+           1       0.80      0.83      0.81       117
+   micro avg       0.81      0.81      0.81       240
+   macro avg       0.81      0.81      0.81       240
+weighted avg       0.81      0.81      0.81       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.78      0.80      0.79       123
+           1       0.78      0.77      0.78       117
+   micro avg       0.78      0.78      0.78       240
+   macro avg       0.78      0.78      0.78       240
+weighted avg       0.78      0.78      0.78       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.74      0.74      0.74        31
+           1       0.72      0.72      0.72        29
+   micro avg       0.73      0.73      0.73        60
+   macro avg       0.73      0.73      0.73        60
+weighted avg       0.73      0.73      0.73        60
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.90      0.78      0.83       123
+           1       0.80      0.91      0.85       117
+   micro avg       0.84      0.84      0.84       240
+   macro avg       0.85      0.84      0.84       240
+weighted avg       0.85      0.84      0.84       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.78      0.68      0.72        31
+           1       0.70      0.79      0.74        29
+   micro avg       0.73      0.73      0.73        60
+   macro avg       0.74      0.74      0.73        60
+weighted avg       0.74      0.73      0.73        60
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.95      0.78      0.86       123
+           1       0.81      0.96      0.88       117
+   micro avg       0.87      0.87      0.87       240
+   macro avg       0.88      0.87      0.87       240
+weighted avg       0.88      0.87      0.87       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The best and equal features:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.82      0.81      0.82       123
+           1       0.81      0.81      0.81       117
+   micro avg       0.81      0.81      0.81       240
+   macro avg       0.81      0.81      0.81       240
+weighted avg       0.81      0.81      0.81       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.73      0.61      0.67        31
+           1       0.65      0.76      0.70        29
+   micro avg       0.68      0.68      0.68        60
+   macro avg       0.69      0.69      0.68        60
+weighted avg       0.69      0.68      0.68        60
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.85      0.86      0.86       123
+           1       0.85      0.85      0.85       117
+   micro avg       0.85      0.85      0.85       240
+   macro avg       0.85      0.85      0.85       240
+weighted avg       0.85      0.85      0.85       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.91      0.86      0.88       123
+           1       0.86      0.91      0.88       117
+   micro avg       0.88      0.88      0.88       240
+   macro avg       0.88      0.88      0.88       240
+weighted avg       0.88      0.88      0.88       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.94      0.80      0.87       123
+           1       0.82      0.95      0.88       117
+   micro avg       0.88      0.88      0.88       240
+   macro avg       0.88      0.88      0.87       240
+weighted avg       0.88      0.88      0.87       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The best and equal features, but removed KNN and RandomForest:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.92      0.82      0.87       123
+           1       0.83      0.92      0.87       117
+   micro avg       0.87      0.87      0.87       240
+   macro avg       0.87      0.87      0.87       240
+weighted avg       0.88      0.87      0.87       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ensembledAveraging 0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ensembledAveraging 0.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ensembledAveraging 0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ensembledAveraging 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.51      1.00      0.68       123
+           1       0.00      0.00      0.00       117
+   micro avg       0.51      0.51      0.51       240
+   macro avg       0.26      0.50      0.34       240
+weighted avg       0.26      0.51      0.35       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.52      1.00      0.68        31
+           1       0.00      0.00      0.00        29
+   micro avg       0.52      0.52      0.52        60
+   macro avg       0.26      0.50      0.34        60
+weighted avg       0.27      0.52      0.35        60
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ensembledAveraging 65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.00      0.00      0.00       123
+           1       0.49      1.00      0.66       117
+   micro avg       0.49      0.49      0.49       240
+   macro avg       0.24      0.50      0.33       240
+weighted avg       0.24      0.49      0.32       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.00      0.00      0.00        31
+           1       0.48      1.00      0.65        29
+   micro avg       0.48      0.48      0.48        60
+   macro avg       0.24      0.50      0.33        60
+weighted avg       0.23      0.48      0.31        60
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ensembledAveraging 0.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.96      0.75      0.84       123
+           1       0.78      0.97      0.87       117
+   micro avg       0.85      0.85      0.85       240
+   macro avg       0.87      0.86      0.85       240
+weighted avg       0.87      0.85      0.85       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.95      0.61      0.75        31
+           1       0.70      0.97      0.81        29
+   micro avg       0.78      0.78      0.78        60
+   macro avg       0.82      0.79      0.78        60
+weighted avg       0.83      0.78      0.78        60
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ensembledAveraging 0.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.99      0.71      0.82       123
+           1       0.76      0.99      0.86       117
+   micro avg       0.85      0.85      0.85       240
+   macro avg       0.88      0.85      0.84       240
+weighted avg       0.88      0.85      0.84       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.94      0.55      0.69        31
+           1       0.67      0.97      0.79        29
+   micro avg       0.75      0.75      0.75        60
+   macro avg       0.81      0.76      0.74        60
+weighted avg       0.81      0.75      0.74        60
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ensembledAveraging 0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.99      0.66      0.79       123
+           1       0.73      0.99      0.84       117
+   micro avg       0.82      0.82      0.82       240
+   macro avg       0.86      0.82      0.82       240
+weighted avg       0.86      0.82      0.82       240
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.94      0.52      0.67        31
+           1       0.65      0.97      0.78        29
+   micro avg       0.73      0.73      0.73        60
+   macro avg       0.80      0.74      0.72        60
+weighted avg       0.80      0.73      0.72        60
 </t>
   </si>
 </sst>
@@ -1299,7 +1530,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1321,6 +1552,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1365,7 +1604,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1380,6 +1619,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1408,10 +1651,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G338"/>
+  <dimension ref="A1:G372"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A325" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A338" activeCellId="0" sqref="A338"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A361" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A372" activeCellId="0" sqref="372:372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9155,8 +9398,8 @@
       </c>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A337" s="1" t="s">
-        <v>82</v>
+      <c r="A337" s="4" t="s">
+        <v>150</v>
       </c>
       <c r="B337" s="1" t="s">
         <v>82</v>
@@ -9177,12 +9420,789 @@
         <v>82</v>
       </c>
     </row>
-    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A338" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B338" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C338" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D338" s="1" t="n">
+        <v>0.812</v>
+      </c>
+      <c r="E338" s="1" t="n">
+        <v>0.717</v>
+      </c>
+      <c r="F338" s="1" t="n">
+        <v>0.813</v>
+      </c>
+      <c r="G338" s="1" t="n">
+        <v>0.719</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A339" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B339" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C339" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D339" s="1" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="E339" s="1" t="n">
+        <v>0.733</v>
+      </c>
+      <c r="F339" s="1" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="G339" s="1" t="n">
+        <v>0.733</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A340" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B340" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C340" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D340" s="1" t="n">
+        <v>0.842</v>
+      </c>
+      <c r="E340" s="1" t="n">
+        <v>0.733</v>
+      </c>
+      <c r="F340" s="1" t="n">
+        <v>0.843</v>
+      </c>
+      <c r="G340" s="1" t="n">
+        <v>0.736</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A341" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B341" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C341" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D341" s="1" t="n">
+        <v>0.933</v>
+      </c>
+      <c r="E341" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="F341" s="1" t="n">
+        <v>0.935</v>
+      </c>
+      <c r="G341" s="1" t="n">
+        <v>0.701</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A342" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B342" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C342" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D342" s="1" t="n">
+        <v>0.867</v>
+      </c>
+      <c r="E342" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F342" s="1" t="n">
+        <v>0.867</v>
+      </c>
+      <c r="G342" s="1" t="n">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A343" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B343" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C343" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D343" s="1" t="n">
+        <v>0.867</v>
+      </c>
+      <c r="E343" s="1" t="n">
+        <v>0.733</v>
+      </c>
+      <c r="F343" s="1" t="n">
+        <v>0.868</v>
+      </c>
+      <c r="G343" s="1" t="n">
+        <v>0.735</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A344" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B344" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C344" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D344" s="1" t="n">
+        <v>0.867</v>
+      </c>
+      <c r="E344" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F344" s="1" t="n">
+        <v>0.869</v>
+      </c>
+      <c r="G344" s="1" t="n">
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A345" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D345" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E345" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F345" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G345" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A346" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B346" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C346" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D346" s="1" t="n">
+        <v>0.812</v>
+      </c>
+      <c r="E346" s="1" t="n">
+        <v>0.683</v>
+      </c>
+      <c r="F346" s="1" t="n">
+        <v>0.812</v>
+      </c>
+      <c r="G346" s="1" t="n">
+        <v>0.686</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A347" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B347" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C347" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D347" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="E347" s="1" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="F347" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="G347" s="1" t="n">
+        <v>0.788</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A348" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B348" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C348" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D348" s="1" t="n">
+        <v>0.854</v>
+      </c>
+      <c r="E348" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F348" s="1" t="n">
+        <v>0.854</v>
+      </c>
+      <c r="G348" s="1" t="n">
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A349" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B349" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C349" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D349" s="1" t="n">
+        <v>0.933</v>
+      </c>
+      <c r="E349" s="1" t="n">
+        <v>0.717</v>
+      </c>
+      <c r="F349" s="1" t="n">
+        <v>0.935</v>
+      </c>
+      <c r="G349" s="1" t="n">
+        <v>0.718</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A350" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B350" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C350" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D350" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="E350" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F350" s="1" t="n">
+        <v>0.872</v>
+      </c>
+      <c r="G350" s="1" t="n">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A351" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B351" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C351" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D351" s="1" t="n">
+        <v>0.883</v>
+      </c>
+      <c r="E351" s="1" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="F351" s="1" t="n">
+        <v>0.884</v>
+      </c>
+      <c r="G351" s="1" t="n">
+        <v>0.771</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A352" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B352" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C352" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D352" s="1" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E352" s="1" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="F352" s="1" t="n">
+        <v>0.877</v>
+      </c>
+      <c r="G352" s="1" t="n">
+        <v>0.772</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A353" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D353" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E353" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F353" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G353" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A354" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B354" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C354" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D354" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="E354" s="1" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="F354" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="G354" s="1" t="n">
+        <v>0.788</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A355" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B355" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C355" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D355" s="1" t="n">
+        <v>0.854</v>
+      </c>
+      <c r="E355" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F355" s="1" t="n">
+        <v>0.854</v>
+      </c>
+      <c r="G355" s="1" t="n">
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A356" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B356" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C356" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D356" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="E356" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F356" s="1" t="n">
+        <v>0.872</v>
+      </c>
+      <c r="G356" s="1" t="n">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A357" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B357" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C357" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D357" s="1" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E357" s="1" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="F357" s="1" t="n">
+        <v>0.876</v>
+      </c>
+      <c r="G357" s="1" t="n">
+        <v>0.771</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A358" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B358" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C358" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D358" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="E358" s="1" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="F358" s="1" t="n">
+        <v>0.872</v>
+      </c>
+      <c r="G358" s="1" t="n">
+        <v>0.772</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A359" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D359" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E359" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F359" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G359" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B360" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C360" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D360" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="E360" s="1" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="F360" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="G360" s="1" t="n">
+        <v>0.788</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B361" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C361" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D361" s="1" t="n">
+        <v>0.854</v>
+      </c>
+      <c r="E361" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F361" s="1" t="n">
+        <v>0.854</v>
+      </c>
+      <c r="G361" s="1" t="n">
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B362" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C362" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D362" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="E362" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F362" s="1" t="n">
+        <v>0.872</v>
+      </c>
+      <c r="G362" s="1" t="n">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B363" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C363" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D363" s="1" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E363" s="1" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="F363" s="1" t="n">
+        <v>0.876</v>
+      </c>
+      <c r="G363" s="1" t="n">
+        <v>0.771</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B364" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C364" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D364" s="1" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E364" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F364" s="1" t="n">
+        <v>0.876</v>
+      </c>
+      <c r="G364" s="1" t="n">
+        <v>0.803</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B365" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C365" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D365" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="E365" s="1" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="F365" s="1" t="n">
+        <v>0.872</v>
+      </c>
+      <c r="G365" s="1" t="n">
+        <v>0.788</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A366" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B366" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C366" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D366" s="1" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="E366" s="1" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="F366" s="1" t="n">
+        <v>0.872</v>
+      </c>
+      <c r="G366" s="1" t="n">
+        <v>0.772</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B367" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C367" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D367" s="1" t="n">
+        <v>0.512</v>
+      </c>
+      <c r="E367" s="1" t="n">
+        <v>0.517</v>
+      </c>
+      <c r="F367" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G367" s="1" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A368" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B368" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C368" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D368" s="1" t="n">
+        <v>0.488</v>
+      </c>
+      <c r="E368" s="1" t="n">
+        <v>0.483</v>
+      </c>
+      <c r="F368" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G368" s="1" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B369" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C369" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D369" s="1" t="n">
+        <v>0.854</v>
+      </c>
+      <c r="E369" s="1" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="F369" s="1" t="n">
+        <v>0.857</v>
+      </c>
+      <c r="G369" s="1" t="n">
+        <v>0.789</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B370" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C370" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D370" s="1" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="E370" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F370" s="1" t="n">
+        <v>0.849</v>
+      </c>
+      <c r="G370" s="1" t="n">
+        <v>0.757</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A371" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B371" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C371" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D371" s="1" t="n">
+        <v>0.821</v>
+      </c>
+      <c r="E371" s="1" t="n">
+        <v>0.733</v>
+      </c>
+      <c r="F371" s="1" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="G371" s="1" t="n">
+        <v>0.741</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>